<commit_message>
readme - pics and readme
</commit_message>
<xml_diff>
--- a/src/fieldupdate/fieldupdate.xlsx
+++ b/src/fieldupdate/fieldupdate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fortuz\GIT\adaptivegame\src\fieldupdate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C06CA1F2-9785-4B42-BE30-4C61B3301BC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73075996-DD1A-42B3-82B4-E245041CACBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1230" yWindow="105" windowWidth="18855" windowHeight="15105" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1230" yWindow="105" windowWidth="16620" windowHeight="15105" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="01_corner" sheetId="4" r:id="rId1"/>
@@ -344,7 +344,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A24D9266-35BD-47B8-AC58-12EFACD6F896}">
   <dimension ref="A1:AN40"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="AP12" sqref="AP12"/>
     </sheetView>
   </sheetViews>
@@ -5254,7 +5254,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89B1B412-1A80-4CF4-A0D0-4883F4BCDDE7}">
   <dimension ref="A1:AN40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="AR9" sqref="AR9"/>
     </sheetView>
   </sheetViews>

</xml_diff>